<commit_message>
Implement mass balance constraints and flow limits In the setup-region portion of the code, I have no implemented the nodal mass balances and the mass flow limits. This reuired small changes to the input files. The most significant change ocurred in the consumer inputs where repitition of consumer for successive years is no longer necessary. The "annual_demand" column was also rebranded as "hourly_demand".
</commit_message>
<xml_diff>
--- a/H2CS2/inputs/input_2region_short.xlsx
+++ b/H2CS2/inputs/input_2region_short.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22a94a39b5425449/Documents/02_School/04_ETH/02_Spring_2023_Semester/06_Case_Study/02_Model/Case-Study-ETH/H2CS2/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funke\OneDrive\Documents\02_School\04_ETH\02_Spring_2023_Semester\06_Case_Study\02_Model\Case-Study-ETH\H2CS2\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{4A406A63-92B2-4734-B287-2E7C5ED84BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{195BDFCF-0B79-44D0-98C1-E13DEF986753}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620A839-78B1-4BCD-B094-6BE7176448C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8904" firstSheet="1" activeTab="1" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="3" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
   <si>
     <t>name</t>
   </si>
@@ -89,9 +89,6 @@
     <t>flow_limit</t>
   </si>
   <si>
-    <t>backbone</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>annual_demand</t>
-  </si>
-  <si>
     <t>kg/year</t>
   </si>
   <si>
@@ -261,6 +255,21 @@
   </si>
   <si>
     <t>vom_scale</t>
+  </si>
+  <si>
+    <t>DE_IT_2030</t>
+  </si>
+  <si>
+    <t>IT_DE_2030</t>
+  </si>
+  <si>
+    <t>DE_IT_2040</t>
+  </si>
+  <si>
+    <t>IT_DE_2040</t>
+  </si>
+  <si>
+    <t>hourly_demand</t>
   </si>
 </sst>
 </file>
@@ -291,12 +300,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -311,10 +326,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,10 +348,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -649,21 +663,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0.06</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -675,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859B5229-E94A-4079-9757-A01BBA7C9852}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="I1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -694,49 +708,49 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -747,10 +761,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -774,16 +788,16 @@
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>9</v>
@@ -791,13 +805,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>2030</v>
@@ -824,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -833,7 +847,7 @@
         <v>0.9</v>
       </c>
       <c r="O3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -841,13 +855,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>2030</v>
@@ -874,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -883,7 +897,7 @@
         <v>0.9</v>
       </c>
       <c r="O4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -891,13 +905,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
       </c>
       <c r="D5">
         <v>2040</v>
@@ -924,7 +938,7 @@
         <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -933,7 +947,7 @@
         <v>0.9</v>
       </c>
       <c r="O5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -941,13 +955,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6">
         <v>2040</v>
@@ -974,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -983,7 +997,7 @@
         <v>0.9</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -997,119 +1011,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAC9B42-355E-42BD-9BE6-F04956BDA26C}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="87" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="14.26171875" customWidth="1"/>
-    <col min="4" max="4" width="23.734375" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="1" max="1" width="14.26171875" customWidth="1"/>
+    <col min="3" max="3" width="23.734375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2030</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>2030</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>2040</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>2000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>2040</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>2000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1122,22 +1090,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97700AB-AD34-4C0B-8BDF-66BBA1C2B828}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="17.3125" customWidth="1"/>
     <col min="5" max="5" width="10.7890625" customWidth="1"/>
     <col min="6" max="6" width="10.5234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1146,21 +1115,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -1179,17 +1148,17 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
         <v>2030</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -1202,17 +1171,17 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
         <v>2030</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -1225,17 +1194,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
         <v>2040</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
       <c r="E5">
         <v>1000</v>
@@ -1248,17 +1217,17 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
         <v>2040</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>1000</v>
@@ -1288,19 +1257,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1311,24 +1280,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
       <c r="D3">
         <v>2030</v>
@@ -1339,13 +1308,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
       </c>
       <c r="D4">
         <v>2040</v>
@@ -1356,13 +1325,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
       <c r="D5">
         <v>2050</v>
@@ -1382,7 +1351,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1397,60 +1366,60 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1458,7 +1427,7 @@
         <v>2030</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <f>1/3</f>
@@ -1466,27 +1435,25 @@
       </c>
       <c r="D3">
         <f ca="1">0.85+0.05*RAND()</f>
-        <v>0.89357054172721595</v>
+        <v>0.85482680346186868</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:G3" ca="1" si="0">0.85+0.05*RAND()</f>
-        <v>0.89447528830851908</v>
+        <v>0.88360930052278208</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87537534221691826</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85612476171051721</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:I8" ca="1" si="1">10 +5*RAND()</f>
-        <v>10.935688350440191</v>
+        <v>13.000849510956051</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="1"/>
-        <v>12.034505584211743</v>
+        <v>11.540423149352307</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1494,7 +1461,7 @@
         <v>2030</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C8" si="2">1/3</f>
@@ -1502,27 +1469,25 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:G8" ca="1" si="3">0.85+0.05*RAND()</f>
-        <v>0.88895167730529645</v>
+        <v>0.86031780185382134</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88799687416123596</v>
+        <v>0.88666159226749142</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.8794165290297723</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88403889954944925</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>14.637437024551764</v>
+        <v>14.140371759442054</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>14.928376855452147</v>
+        <v>11.990867837332814</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1530,7 +1495,7 @@
         <v>2030</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <f t="shared" si="2"/>
@@ -1538,27 +1503,25 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85937307094093374</v>
+        <v>0.89971175431302564</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="3"/>
-        <v>0.86236744282095756</v>
+        <v>0.86278719405928783</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.8602133915217397</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88391021021670024</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>10.863402491993185</v>
+        <v>10.32036819419551</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>10.204114718141122</v>
+        <v>11.059348797284697</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1566,7 +1529,7 @@
         <v>2040</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
@@ -1574,27 +1537,25 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87920347041800673</v>
+        <v>0.87625001135843916</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="3"/>
-        <v>0.86102919560307767</v>
+        <v>0.89955985414701267</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88384609466515363</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.86754300164657661</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>14.685022030123568</v>
+        <v>13.993902092369925</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>13.191338439890631</v>
+        <v>11.785651668492081</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1602,7 +1563,7 @@
         <v>2040</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
@@ -1610,27 +1571,25 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>0.86567142141431108</v>
+        <v>0.87580215602582268</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8691689150707711</v>
+        <v>0.86903941878368307</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.87710445763268607</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.87388703448351768</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>10.236526055553146</v>
+        <v>14.782743636773997</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>12.61981677274038</v>
+        <v>10.373121302243071</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1638,7 +1597,7 @@
         <v>2040</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
@@ -1646,27 +1605,25 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.89362488106449023</v>
+        <v>0.88691336825283473</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88856224883318435</v>
+        <v>0.88068049419960082</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.8516040833327122</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.87001706862143813</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>11.533004083850972</v>
+        <v>13.873433296675284</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>12.748746108402186</v>
+        <v>11.782346785694081</v>
       </c>
     </row>
   </sheetData>
@@ -1694,40 +1651,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1738,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -1759,21 +1716,21 @@
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>2030</v>
@@ -1809,10 +1766,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2040</v>
@@ -1847,10 +1804,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>2050</v>

</xml_diff>

<commit_message>
Add Outputs The model now saves the values of the primal and dual variables to an output spreadsheet, located in the "./H2CS2/output/" folder.
</commit_message>
<xml_diff>
--- a/H2CS2/inputs/input_2region_short.xlsx
+++ b/H2CS2/inputs/input_2region_short.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funke\OneDrive\Documents\02_School\04_ETH\02_Spring_2023_Semester\06_Case_Study\02_Model\Case-Study-ETH\H2CS2\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22a94a39b5425449/Documents/02_School/04_ETH/02_Spring_2023_Semester/06_Case_Study/02_Model/Case-Study-ETH/H2CS2/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620A839-78B1-4BCD-B094-6BE7176448C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{2620A839-78B1-4BCD-B094-6BE7176448C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE89A68B-FB76-4329-A584-C1E719CD738D}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="3" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
+    <workbookView xWindow="17400" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
   <si>
     <t>name</t>
   </si>
@@ -155,12 +155,6 @@
     <t>{1 = newly built, 0 existing}</t>
   </si>
   <si>
-    <t>$/(kg/yr)</t>
-  </si>
-  <si>
-    <t>$/(kg/year)/yr</t>
-  </si>
-  <si>
     <t>$/kg</t>
   </si>
   <si>
@@ -270,13 +264,22 @@
   </si>
   <si>
     <t>hourly_demand</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>$/(kg/hr)/yr</t>
+  </si>
+  <si>
+    <t>$/(kg/hr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,19 +302,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -323,19 +327,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -348,6 +352,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -650,7 +658,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -673,11 +681,12 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>0.06</v>
+      <c r="B2" s="3">
+        <f>10%</f>
+        <v>0.1</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -689,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859B5229-E94A-4079-9757-A01BBA7C9852}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -701,7 +710,9 @@
     <col min="7" max="8" width="18.83984375" customWidth="1"/>
     <col min="9" max="9" width="12.41796875" customWidth="1"/>
     <col min="10" max="10" width="26.26171875" customWidth="1"/>
-    <col min="11" max="13" width="13.26171875" customWidth="1"/>
+    <col min="11" max="11" width="13.26171875" customWidth="1"/>
+    <col min="12" max="12" width="20.20703125" customWidth="1"/>
+    <col min="13" max="13" width="13.26171875" customWidth="1"/>
     <col min="14" max="15" width="24.578125" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
   </cols>
@@ -723,34 +734,34 @@
         <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -788,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>27</v>
@@ -797,7 +808,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>9</v>
@@ -805,13 +816,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>2030</v>
@@ -820,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -829,25 +840,25 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>10</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -855,13 +866,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>2030</v>
@@ -882,22 +893,22 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -905,13 +916,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>2040</v>
@@ -923,31 +934,31 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>20</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>10</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -955,13 +966,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>2040</v>
@@ -973,31 +984,31 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <v>20</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>11</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1014,7 +1025,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="87" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1024,60 +1035,60 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>64</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1090,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97700AB-AD34-4C0B-8BDF-66BBA1C2B828}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1149,7 +1160,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>2030</v>
@@ -1164,15 +1175,15 @@
         <v>1000</v>
       </c>
       <c r="F3">
-        <v>0.3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>2030</v>
@@ -1187,15 +1198,15 @@
         <v>1000</v>
       </c>
       <c r="F4">
-        <v>0.3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>2040</v>
@@ -1210,15 +1221,15 @@
         <v>1000</v>
       </c>
       <c r="F5">
-        <v>0.25</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G5">
-        <v>500</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>2040</v>
@@ -1233,10 +1244,10 @@
         <v>1000</v>
       </c>
       <c r="F6">
-        <v>0.25</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G6">
-        <v>500</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1350,16 +1361,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC100551-67EA-4544-94EF-22E0A8082156}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="4" max="4" width="24.3125" customWidth="1"/>
     <col min="5" max="5" width="17.89453125" customWidth="1"/>
-    <col min="6" max="6" width="14.41796875" customWidth="1"/>
-    <col min="7" max="7" width="12.26171875" customWidth="1"/>
+    <col min="6" max="6" width="19.68359375" customWidth="1"/>
+    <col min="7" max="7" width="17.7890625" customWidth="1"/>
     <col min="8" max="8" width="29.20703125" customWidth="1"/>
     <col min="9" max="9" width="31.20703125" customWidth="1"/>
   </cols>
@@ -1372,25 +1383,25 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1398,28 +1409,28 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1430,30 +1441,25 @@
         <v>26</v>
       </c>
       <c r="C3">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D3">
-        <f ca="1">0.85+0.05*RAND()</f>
-        <v>0.85482680346186868</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:G3" ca="1" si="0">0.85+0.05*RAND()</f>
-        <v>0.88360930052278208</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:I8" ca="1" si="1">10 +5*RAND()</f>
-        <v>13.000849510956051</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.540423149352307</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1461,19 +1467,16 @@
         <v>2030</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="2">1/3</f>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:G8" ca="1" si="3">0.85+0.05*RAND()</f>
-        <v>0.86031780185382134</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88666159226749142</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1482,12 +1485,10 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="1"/>
-        <v>14.140371759442054</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.990867837332814</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1495,33 +1496,28 @@
         <v>2030</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.89971175431302564</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.86278719405928783</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="1"/>
-        <v>10.32036819419551</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.059348797284697</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1532,30 +1528,25 @@
         <v>26</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.87625001135843916</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.89955985414701267</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="1"/>
-        <v>13.993902092369925</v>
+        <v>0.5</v>
       </c>
       <c r="I6">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.785651668492081</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1563,33 +1554,28 @@
         <v>2040</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.87580215602582268</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.86903941878368307</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="1"/>
-        <v>14.782743636773997</v>
+        <v>0.5</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="1"/>
-        <v>10.373121302243071</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1597,37 +1583,33 @@
         <v>2040</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>1000</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88691336825283473</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.88068049419960082</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="1"/>
-        <v>13.873433296675284</v>
+        <v>0.5</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="1"/>
-        <v>11.782346785694081</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1660,22 +1642,22 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J1" t="s">
         <v>33</v>
@@ -1716,18 +1698,18 @@
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1766,7 +1748,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1804,7 +1786,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Add electricity prices and gas prices Variable costs are now split into non-fuel variable costs and gas/electricity costs. Hourly electricity and gas prices are now taken as a explicit input to the model. See the input spreadsheet for details.
</commit_message>
<xml_diff>
--- a/H2CS2/inputs/input_2region_short.xlsx
+++ b/H2CS2/inputs/input_2region_short.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22a94a39b5425449/Documents/02_School/04_ETH/02_Spring_2023_Semester/06_Case_Study/02_Model/Case-Study-ETH/H2CS2/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{2620A839-78B1-4BCD-B094-6BE7176448C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE89A68B-FB76-4329-A584-C1E719CD738D}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{2620A839-78B1-4BCD-B094-6BE7176448C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6685DBC2-64E8-483A-9605-AC9C2F6F1BBB}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
+    <workbookView xWindow="17400" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{B45309CD-61A4-4A28-84F6-A1F6AFA13388}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="6" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="consumer" sheetId="3" r:id="rId3"/>
     <sheet name="transportation" sheetId="1" r:id="rId4"/>
     <sheet name="policy" sheetId="5" r:id="rId5"/>
-    <sheet name="time" sheetId="4" r:id="rId6"/>
-    <sheet name="storage" sheetId="7" r:id="rId7"/>
+    <sheet name="electricity_price" sheetId="8" r:id="rId6"/>
+    <sheet name="gas_price" sheetId="9" r:id="rId7"/>
+    <sheet name="time" sheetId="4" r:id="rId8"/>
+    <sheet name="storage" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -125,9 +127,6 @@
     <t>jan</t>
   </si>
   <si>
-    <t>fuel_cost</t>
-  </si>
-  <si>
     <t>Eur/kg/km</t>
   </si>
   <si>
@@ -236,21 +235,12 @@
     <t>DE_Demand_Scale</t>
   </si>
   <si>
-    <t>DE_electrolyzer_VOM</t>
-  </si>
-  <si>
-    <t>IT_electrolyzer_VOM</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
     <t>availability_scale</t>
   </si>
   <si>
-    <t>vom_scale</t>
-  </si>
-  <si>
     <t>DE_IT_2030</t>
   </si>
   <si>
@@ -273,6 +263,27 @@
   </si>
   <si>
     <t>$/(kg/hr)</t>
+  </si>
+  <si>
+    <t>gas_requirement</t>
+  </si>
+  <si>
+    <t>electricity_requirement</t>
+  </si>
+  <si>
+    <t>kwh/kg</t>
+  </si>
+  <si>
+    <t>mmbtu/kg</t>
+  </si>
+  <si>
+    <t>nonfuel_variable_cost</t>
+  </si>
+  <si>
+    <t>$/kWh</t>
+  </si>
+  <si>
+    <t>$/mmbtu</t>
   </si>
 </sst>
 </file>
@@ -674,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -686,7 +697,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -698,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859B5229-E94A-4079-9757-A01BBA7C9852}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="E1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -710,58 +721,60 @@
     <col min="7" max="8" width="18.83984375" customWidth="1"/>
     <col min="9" max="9" width="12.41796875" customWidth="1"/>
     <col min="10" max="10" width="26.26171875" customWidth="1"/>
-    <col min="11" max="11" width="13.26171875" customWidth="1"/>
-    <col min="12" max="12" width="20.20703125" customWidth="1"/>
-    <col min="13" max="13" width="13.26171875" customWidth="1"/>
+    <col min="11" max="12" width="20.20703125" customWidth="1"/>
+    <col min="13" max="13" width="19.89453125" customWidth="1"/>
     <col min="14" max="15" width="24.578125" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -796,19 +809,19 @@
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>9</v>
@@ -816,13 +829,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>2030</v>
@@ -846,10 +859,10 @@
         <v>10</v>
       </c>
       <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>64</v>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -858,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -866,13 +879,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>2030</v>
@@ -896,10 +909,10 @@
         <v>20</v>
       </c>
       <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -908,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -916,13 +929,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>2040</v>
@@ -946,10 +959,10 @@
         <v>10</v>
       </c>
       <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>64</v>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -958,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -966,13 +979,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>2040</v>
@@ -996,10 +1009,10 @@
         <v>11</v>
       </c>
       <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1008,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1037,16 +1050,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1057,15 +1070,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1074,12 +1087,12 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1088,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1127,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
@@ -1126,13 +1139,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1160,7 +1173,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>2030</v>
@@ -1183,7 +1196,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>2030</v>
@@ -1206,7 +1219,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>2040</v>
@@ -1229,7 +1242,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>2040</v>
@@ -1268,19 +1281,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="11.7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1358,11 +1371,266 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03903C7-1A75-4899-99E1-0F471DE44DCA}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2030</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2030</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2030</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2040</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2040</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2040</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FCACF-C696-4CAF-9099-6DD409076FA2}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2030</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2030</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2030</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2040</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2040</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2040</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC100551-67EA-4544-94EF-22E0A8082156}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1371,11 +1639,9 @@
     <col min="5" max="5" width="17.89453125" customWidth="1"/>
     <col min="6" max="6" width="19.68359375" customWidth="1"/>
     <col min="7" max="7" width="17.7890625" customWidth="1"/>
-    <col min="8" max="8" width="29.20703125" customWidth="1"/>
-    <col min="9" max="9" width="31.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1383,57 +1649,45 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2030</v>
       </c>
@@ -1455,19 +1709,13 @@
       <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2030</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1000</v>
@@ -1484,19 +1732,13 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="I4">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2030</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1000</v>
@@ -1513,14 +1755,8 @@
       <c r="G5">
         <v>0.75</v>
       </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-      <c r="I5">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2040</v>
       </c>
@@ -1542,19 +1778,13 @@
       <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6">
-        <v>0.5</v>
-      </c>
-      <c r="I6">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>2040</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>1000</v>
@@ -1571,19 +1801,13 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7">
-        <v>0.5</v>
-      </c>
-      <c r="I7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>2040</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -1599,12 +1823,6 @@
       </c>
       <c r="G8">
         <v>0.75</v>
-      </c>
-      <c r="H8">
-        <v>0.5</v>
-      </c>
-      <c r="I8">
-        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +1831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A06BFA3-71C2-4E46-AF9F-2CC7C04ED2E6}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1633,7 +1851,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1642,31 +1860,31 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1698,18 +1916,18 @@
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1748,7 +1966,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1786,7 +2004,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>

</xml_diff>